<commit_message>
update tuvung from 1 to 5
</commit_message>
<xml_diff>
--- a/TuVung/Lesson1/tuvung.xlsx
+++ b/TuVung/Lesson1/tuvung.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\01_LearningJapaneseWebProject\TuVung\Lesson1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F1EDC59-FD4D-4BF3-BFE2-5680A5EED490}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B673120-AC02-4C08-A559-1BA68246F2A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5595" yWindow="2340" windowWidth="21495" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -300,10 +300,10 @@
     <t>Ý</t>
   </si>
   <si>
-    <t>第二課</t>
-  </si>
-  <si>
     <t>subjapanese</t>
+  </si>
+  <si>
+    <t>第ー課</t>
   </si>
 </sst>
 </file>
@@ -658,7 +658,7 @@
   <dimension ref="A1:D364"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -676,7 +676,7 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
@@ -684,7 +684,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>

</xml_diff>